<commit_message>
adding a label 2 show the search statuse
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -731,6 +731,13 @@
       <c r="E11" t="inlineStr">
         <is>
           <t>"09987786786"</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>mailto:aram@gamil.com</t>
         </is>
       </c>
     </row>

</xml_diff>